<commit_message>
Color scheme and word layour changed
</commit_message>
<xml_diff>
--- a/TERM TEMPLATE.xlsx
+++ b/TERM TEMPLATE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\visag\TERM SUBJECT ANALYSIS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F761E9-2CC1-4EE8-ABBF-524F026B6110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D8612F-7BD7-4331-AA91-CCE4D2D5BEB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{219C4AAB-400E-4B09-B933-C56F029F548B}"/>
   </bookViews>
@@ -672,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADC5ECD1-A5BD-45FF-BA4D-3421F446993F}">
   <dimension ref="A1:J95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="A95" sqref="A95"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="M86" sqref="M86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,31 +739,28 @@
         <v>37</v>
       </c>
       <c r="B7">
-        <v>56.608108108108105</v>
-      </c>
-      <c r="C7">
-        <v>5</v>
+        <v>61.418604651162788</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E7">
+        <v>13</v>
+      </c>
+      <c r="F7">
+        <v>23</v>
+      </c>
+      <c r="G7">
+        <v>18</v>
+      </c>
+      <c r="H7">
+        <v>17</v>
+      </c>
+      <c r="I7">
         <v>9</v>
       </c>
-      <c r="F7">
-        <v>20</v>
-      </c>
-      <c r="G7">
-        <v>19</v>
-      </c>
-      <c r="H7">
-        <v>18</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
       <c r="J7">
-        <v>74</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -771,31 +768,31 @@
         <v>38</v>
       </c>
       <c r="B8">
-        <v>60.076677316293932</v>
+        <v>49.666666666666664</v>
       </c>
       <c r="C8">
+        <v>31</v>
+      </c>
+      <c r="D8">
         <v>37</v>
       </c>
-      <c r="D8">
-        <v>15</v>
-      </c>
       <c r="E8">
-        <v>11</v>
+        <v>62</v>
       </c>
       <c r="F8">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G8">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="H8">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="I8">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="J8">
-        <v>313</v>
+        <v>270</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -803,31 +800,31 @@
         <v>13</v>
       </c>
       <c r="B9">
-        <v>70.645994832041339</v>
+        <v>53.825842696629216</v>
       </c>
       <c r="C9">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="D9">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="E9">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="F9">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="G9">
-        <v>34</v>
+        <v>121</v>
       </c>
       <c r="H9">
-        <v>85</v>
+        <v>49</v>
       </c>
       <c r="I9">
-        <v>203</v>
+        <v>22</v>
       </c>
       <c r="J9">
-        <v>387</v>
+        <v>356</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -835,31 +832,31 @@
         <v>14</v>
       </c>
       <c r="B10">
-        <v>66.196382428940566</v>
+        <v>50.724719101123597</v>
       </c>
       <c r="C10">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="D10">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="E10">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="F10">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="G10">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="H10">
-        <v>102</v>
+        <v>49</v>
       </c>
       <c r="I10">
-        <v>132</v>
+        <v>16</v>
       </c>
       <c r="J10">
-        <v>387</v>
+        <v>356</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -867,31 +864,28 @@
         <v>15</v>
       </c>
       <c r="B11">
-        <v>54.581469648562297</v>
+        <v>44.985185185185188</v>
       </c>
       <c r="C11">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="D11">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="E11">
-        <v>49</v>
+        <v>97</v>
       </c>
       <c r="F11">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="G11">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="H11">
-        <v>56</v>
-      </c>
-      <c r="I11">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="J11">
-        <v>313</v>
+        <v>270</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -899,31 +893,31 @@
         <v>16</v>
       </c>
       <c r="B12">
-        <v>60.270270270270274</v>
+        <v>51.325581395348834</v>
       </c>
       <c r="C12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E12">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="F12">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G12">
         <v>16</v>
       </c>
       <c r="H12">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I12">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="J12">
-        <v>74</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -931,31 +925,31 @@
         <v>17</v>
       </c>
       <c r="B13">
-        <v>62.470284237726098</v>
+        <v>63.233146067415731</v>
       </c>
       <c r="C13">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="D13">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E13">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="F13">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="G13">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="H13">
-        <v>160</v>
+        <v>51</v>
       </c>
       <c r="I13">
-        <v>38</v>
+        <v>85</v>
       </c>
       <c r="J13">
-        <v>387</v>
+        <v>356</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -963,31 +957,28 @@
         <v>18</v>
       </c>
       <c r="B14">
-        <v>31.322997416020673</v>
+        <v>22.789325842696631</v>
       </c>
       <c r="C14">
-        <v>156</v>
+        <v>259</v>
       </c>
       <c r="D14">
-        <v>127</v>
+        <v>51</v>
       </c>
       <c r="E14">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="F14">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G14">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H14">
-        <v>4</v>
-      </c>
-      <c r="I14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J14">
-        <v>387</v>
+        <v>356</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -995,31 +986,28 @@
         <v>19</v>
       </c>
       <c r="B15">
-        <v>42.355670103092784</v>
+        <v>37.682584269662918</v>
       </c>
       <c r="C15">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="D15">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="E15">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F15">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="G15">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="H15">
-        <v>12</v>
-      </c>
-      <c r="I15">
         <v>1</v>
       </c>
       <c r="J15">
-        <v>388</v>
+        <v>356</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1027,31 +1015,31 @@
         <v>20</v>
       </c>
       <c r="B16">
-        <v>57.578811369509047</v>
+        <v>49.665730337078649</v>
       </c>
       <c r="C16">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="D16">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E16">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="F16">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="G16">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="H16">
-        <v>88</v>
+        <v>58</v>
       </c>
       <c r="I16">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="J16">
-        <v>387</v>
+        <v>356</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1059,31 +1047,31 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>60.808785529715763</v>
+        <v>55.238764044943821</v>
       </c>
       <c r="C17">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="D17">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E17">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="F17">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="G17">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="H17">
-        <v>204</v>
+        <v>69</v>
       </c>
       <c r="I17">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="J17">
-        <v>387</v>
+        <v>356</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1128,31 +1116,31 @@
         <v>41</v>
       </c>
       <c r="B21">
-        <v>47.535714285714285</v>
+        <v>40.689189189189186</v>
       </c>
       <c r="C21">
+        <v>16</v>
+      </c>
+      <c r="D21">
+        <v>21</v>
+      </c>
+      <c r="E21">
+        <v>20</v>
+      </c>
+      <c r="F21">
         <v>8</v>
       </c>
-      <c r="D21">
-        <v>9</v>
-      </c>
-      <c r="E21">
-        <v>11</v>
-      </c>
-      <c r="F21">
-        <v>13</v>
-      </c>
       <c r="G21">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H21">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J21">
-        <v>56</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1160,22 +1148,31 @@
         <v>39</v>
       </c>
       <c r="B22">
-        <v>60.44</v>
+        <v>59.363636363636367</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>16</v>
       </c>
       <c r="F22">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="G22">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="H22">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="I22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J22">
-        <v>75</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1183,28 +1180,31 @@
         <v>40</v>
       </c>
       <c r="B23">
-        <v>73.319018404907979</v>
+        <v>54.884848484848483</v>
       </c>
       <c r="C23">
+        <v>24</v>
+      </c>
+      <c r="D23">
+        <v>37</v>
+      </c>
+      <c r="E23">
+        <v>38</v>
+      </c>
+      <c r="F23">
+        <v>74</v>
+      </c>
+      <c r="G23">
+        <v>102</v>
+      </c>
+      <c r="H23">
+        <v>40</v>
+      </c>
+      <c r="I23">
         <v>15</v>
       </c>
-      <c r="E23">
-        <v>4</v>
-      </c>
-      <c r="F23">
-        <v>17</v>
-      </c>
-      <c r="G23">
-        <v>47</v>
-      </c>
-      <c r="H23">
-        <v>100</v>
-      </c>
-      <c r="I23">
-        <v>143</v>
-      </c>
       <c r="J23">
-        <v>326</v>
+        <v>330</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1212,22 +1212,25 @@
         <v>36</v>
       </c>
       <c r="B24">
-        <v>30.642857142857142</v>
+        <v>27.745454545454546</v>
       </c>
       <c r="C24">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="D24">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E24">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F24">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="G24">
+        <v>2</v>
       </c>
       <c r="J24">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1235,28 +1238,22 @@
         <v>42</v>
       </c>
       <c r="B25">
-        <v>52.208333333333336</v>
+        <v>23.306818181818183</v>
       </c>
       <c r="C25">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="D25">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="E25">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F25">
-        <v>16</v>
-      </c>
-      <c r="G25">
-        <v>17</v>
-      </c>
-      <c r="H25">
         <v>2</v>
       </c>
       <c r="J25">
-        <v>48</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1264,28 +1261,31 @@
         <v>43</v>
       </c>
       <c r="B26">
-        <v>39.172413793103445</v>
+        <v>32.588888888888889</v>
       </c>
       <c r="C26">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="D26">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E26">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="F26">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="G26">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H26">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="I26">
+        <v>2</v>
       </c>
       <c r="J26">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1293,25 +1293,28 @@
         <v>44</v>
       </c>
       <c r="B27">
-        <v>72</v>
+        <v>68.727272727272734</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F27">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G27">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H27">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="I27">
         <v>8</v>
       </c>
       <c r="J27">
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1319,28 +1322,31 @@
         <v>35</v>
       </c>
       <c r="B28">
-        <v>76.898876404494388</v>
+        <v>62.262500000000003</v>
       </c>
       <c r="C28">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
       </c>
       <c r="E28">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F28">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G28">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="H28">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="I28">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="J28">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -1348,31 +1354,31 @@
         <v>45</v>
       </c>
       <c r="B29">
-        <v>62.203076923076921</v>
+        <v>49.369696969696967</v>
       </c>
       <c r="C29">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="D29">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="E29">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="F29">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="G29">
-        <v>104</v>
+        <v>47</v>
       </c>
       <c r="H29">
-        <v>101</v>
+        <v>31</v>
       </c>
       <c r="I29">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="J29">
-        <v>325</v>
+        <v>330</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -1380,28 +1386,31 @@
         <v>46</v>
       </c>
       <c r="B30">
-        <v>65.693333333333328</v>
+        <v>52.079545454545453</v>
       </c>
       <c r="C30">
         <v>4</v>
       </c>
+      <c r="D30">
+        <v>6</v>
+      </c>
       <c r="E30">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="F30">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="G30">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="H30">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="I30">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="J30">
-        <v>75</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -1409,31 +1418,25 @@
         <v>47</v>
       </c>
       <c r="B31">
-        <v>43.209302325581397</v>
+        <v>28.238993710691823</v>
       </c>
       <c r="C31">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="D31">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E31">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F31">
-        <v>25</v>
-      </c>
-      <c r="G31">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="H31">
-        <v>9</v>
-      </c>
-      <c r="I31">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="J31">
-        <v>172</v>
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -1441,31 +1444,31 @@
         <v>48</v>
       </c>
       <c r="B32">
-        <v>54.155172413793103</v>
+        <v>50.388235294117649</v>
       </c>
       <c r="C32">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D32">
+        <v>19</v>
+      </c>
+      <c r="E32">
+        <v>52</v>
+      </c>
+      <c r="F32">
+        <v>37</v>
+      </c>
+      <c r="G32">
+        <v>30</v>
+      </c>
+      <c r="H32">
         <v>18</v>
       </c>
-      <c r="E32">
-        <v>31</v>
-      </c>
-      <c r="F32">
-        <v>35</v>
-      </c>
-      <c r="G32">
-        <v>42</v>
-      </c>
-      <c r="H32">
-        <v>24</v>
-      </c>
       <c r="I32">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="J32">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -1473,31 +1476,31 @@
         <v>49</v>
       </c>
       <c r="B33">
-        <v>65.564999999999998</v>
+        <v>46.380382775119614</v>
       </c>
       <c r="C33">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="D33">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="E33">
-        <v>27</v>
+        <v>98</v>
       </c>
       <c r="F33">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="G33">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="H33">
-        <v>100</v>
+        <v>37</v>
       </c>
       <c r="I33">
-        <v>99</v>
+        <v>12</v>
       </c>
       <c r="J33">
-        <v>400</v>
+        <v>418</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -1505,28 +1508,28 @@
         <v>50</v>
       </c>
       <c r="B34">
-        <v>37.107843137254903</v>
+        <v>30.473684210526315</v>
       </c>
       <c r="C34">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="D34">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E34">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="F34">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G34">
-        <v>9</v>
-      </c>
-      <c r="H34">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
       </c>
       <c r="J34">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -1534,22 +1537,31 @@
         <v>51</v>
       </c>
       <c r="B35">
-        <v>27.480314960629922</v>
+        <v>35.952029520295206</v>
       </c>
       <c r="C35">
-        <v>144</v>
+        <v>85</v>
       </c>
       <c r="D35">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E35">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="F35">
-        <v>8</v>
+        <v>37</v>
+      </c>
+      <c r="G35">
+        <v>14</v>
+      </c>
+      <c r="H35">
+        <v>2</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
       </c>
       <c r="J35">
-        <v>254</v>
+        <v>271</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -1557,22 +1569,25 @@
         <v>52</v>
       </c>
       <c r="B36">
-        <v>26.736842105263158</v>
+        <v>27.988636363636363</v>
       </c>
       <c r="C36">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="D36">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E36">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F36">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
       </c>
       <c r="J36">
-        <v>76</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -1580,28 +1595,22 @@
         <v>32</v>
       </c>
       <c r="B37">
-        <v>79.583333333333329</v>
-      </c>
-      <c r="D37">
-        <v>2</v>
-      </c>
-      <c r="E37">
-        <v>1</v>
+        <v>80.615384615384613</v>
       </c>
       <c r="F37">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G37">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H37">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I37">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J37">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -1609,31 +1618,31 @@
         <v>33</v>
       </c>
       <c r="B38">
-        <v>54.592592592592595</v>
+        <v>51.846153846153847</v>
       </c>
       <c r="C38">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E38">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F38">
         <v>4</v>
       </c>
       <c r="G38">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H38">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I38">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J38">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -1641,28 +1650,25 @@
         <v>34</v>
       </c>
       <c r="B39">
-        <v>73</v>
+        <v>45.75</v>
       </c>
       <c r="C39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
-      <c r="F39">
+      <c r="E39">
         <v>2</v>
       </c>
       <c r="G39">
-        <v>3</v>
-      </c>
-      <c r="H39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I39">
+        <v>1</v>
+      </c>
+      <c r="J39">
         <v>8</v>
-      </c>
-      <c r="J39">
-        <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -1670,25 +1676,28 @@
         <v>53</v>
       </c>
       <c r="B40">
-        <v>33.117647058823529</v>
+        <v>29.482758620689655</v>
       </c>
       <c r="C40">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="D40">
         <v>15</v>
       </c>
       <c r="E40">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="F40">
         <v>4</v>
       </c>
       <c r="G40">
+        <v>2</v>
+      </c>
+      <c r="H40">
         <v>1</v>
       </c>
       <c r="J40">
-        <v>51</v>
+        <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -1696,28 +1705,22 @@
         <v>54</v>
       </c>
       <c r="B41">
-        <v>33.585714285714289</v>
+        <v>20.254237288135592</v>
       </c>
       <c r="C41">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="D41">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E41">
-        <v>15</v>
-      </c>
-      <c r="F41">
-        <v>8</v>
-      </c>
-      <c r="G41">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H41">
         <v>1</v>
       </c>
       <c r="J41">
-        <v>70</v>
+        <v>59</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -1725,28 +1728,25 @@
         <v>55</v>
       </c>
       <c r="B42">
-        <v>50.721518987341774</v>
+        <v>43.161764705882355</v>
       </c>
       <c r="C42">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D42">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="E42">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="F42">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="G42">
-        <v>14</v>
-      </c>
-      <c r="H42">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J42">
-        <v>79</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -1754,28 +1754,28 @@
         <v>56</v>
       </c>
       <c r="B43">
-        <v>46.061032863849768</v>
+        <v>36.232067510548525</v>
       </c>
       <c r="C43">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="D43">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="E43">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="F43">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="G43">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="H43">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="J43">
-        <v>213</v>
+        <v>237</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -1820,25 +1820,31 @@
         <v>57</v>
       </c>
       <c r="B47">
-        <v>68.875</v>
+        <v>48.676470588235297</v>
+      </c>
+      <c r="C47">
+        <v>5</v>
+      </c>
+      <c r="D47">
+        <v>4</v>
       </c>
       <c r="E47">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F47">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G47">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H47">
         <v>3</v>
       </c>
       <c r="I47">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J47">
-        <v>16</v>
+        <v>34</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -1846,22 +1852,28 @@
         <v>58</v>
       </c>
       <c r="B48">
-        <v>66.518518518518519</v>
+        <v>56.153846153846153</v>
+      </c>
+      <c r="C48">
+        <v>2</v>
+      </c>
+      <c r="D48">
+        <v>4</v>
+      </c>
+      <c r="E48">
+        <v>5</v>
       </c>
       <c r="F48">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="G48">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="H48">
-        <v>15</v>
-      </c>
-      <c r="I48">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="J48">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -1869,28 +1881,31 @@
         <v>59</v>
       </c>
       <c r="B49">
-        <v>75.581589958159</v>
+        <v>57.576000000000001</v>
       </c>
       <c r="C49">
         <v>4</v>
       </c>
+      <c r="D49">
+        <v>14</v>
+      </c>
       <c r="E49">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="F49">
-        <v>6</v>
+        <v>88</v>
       </c>
       <c r="G49">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H49">
-        <v>91</v>
+        <v>31</v>
       </c>
       <c r="I49">
-        <v>102</v>
+        <v>22</v>
       </c>
       <c r="J49">
-        <v>239</v>
+        <v>250</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
@@ -1898,22 +1913,25 @@
         <v>60</v>
       </c>
       <c r="B50">
-        <v>36.0625</v>
+        <v>42.071428571428569</v>
       </c>
       <c r="C50">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D50">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E50">
-        <v>4</v>
+        <v>10</v>
+      </c>
+      <c r="F50">
+        <v>6</v>
       </c>
       <c r="G50">
         <v>1</v>
       </c>
       <c r="J50">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
@@ -1921,28 +1939,19 @@
         <v>61</v>
       </c>
       <c r="B51">
-        <v>49.673913043478258</v>
+        <v>25.068965517241381</v>
       </c>
       <c r="C51">
+        <v>18</v>
+      </c>
+      <c r="D51">
         <v>7</v>
       </c>
-      <c r="D51">
-        <v>19</v>
-      </c>
       <c r="E51">
-        <v>44</v>
-      </c>
-      <c r="F51">
-        <v>37</v>
-      </c>
-      <c r="G51">
-        <v>18</v>
-      </c>
-      <c r="H51">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="J51">
-        <v>138</v>
+        <v>29</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
@@ -1950,28 +1959,31 @@
         <v>62</v>
       </c>
       <c r="B52">
-        <v>49</v>
+        <v>46.412698412698411</v>
       </c>
       <c r="C52">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D52">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E52">
+        <v>6</v>
+      </c>
+      <c r="F52">
+        <v>16</v>
+      </c>
+      <c r="G52">
         <v>9</v>
       </c>
-      <c r="F52">
-        <v>7</v>
-      </c>
-      <c r="G52">
-        <v>4</v>
-      </c>
       <c r="H52">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="I52">
+        <v>1</v>
       </c>
       <c r="J52">
-        <v>27</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
@@ -1979,19 +1991,25 @@
         <v>63</v>
       </c>
       <c r="B53">
-        <v>81</v>
+        <v>66.444444444444443</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="F53">
+        <v>3</v>
       </c>
       <c r="G53">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H53">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I53">
         <v>4</v>
       </c>
       <c r="J53">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
@@ -1999,31 +2017,31 @@
         <v>31</v>
       </c>
       <c r="B54">
-        <v>67.63333333333334</v>
+        <v>69</v>
       </c>
       <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
         <v>3</v>
       </c>
-      <c r="D54">
-        <v>2</v>
-      </c>
-      <c r="E54">
-        <v>10</v>
-      </c>
       <c r="F54">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G54">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="H54">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="I54">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="J54">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
@@ -2031,31 +2049,31 @@
         <v>64</v>
       </c>
       <c r="B55">
-        <v>62.686192468619247</v>
+        <v>62.856000000000002</v>
       </c>
       <c r="C55">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D55">
         <v>6</v>
       </c>
       <c r="E55">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="F55">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="G55">
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="H55">
-        <v>87</v>
+        <v>51</v>
       </c>
       <c r="I55">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="J55">
-        <v>239</v>
+        <v>250</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
@@ -2063,19 +2081,28 @@
         <v>65</v>
       </c>
       <c r="B56">
-        <v>84.962962962962962</v>
+        <v>56.615384615384613</v>
+      </c>
+      <c r="D56">
+        <v>2</v>
+      </c>
+      <c r="E56">
+        <v>7</v>
+      </c>
+      <c r="F56">
+        <v>26</v>
       </c>
       <c r="G56">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H56">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="I56">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="J56">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
@@ -2083,31 +2110,28 @@
         <v>66</v>
       </c>
       <c r="B57">
-        <v>40.205882352941174</v>
+        <v>37.261194029850749</v>
       </c>
       <c r="C57">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="D57">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="E57">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="F57">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="G57">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H57">
-        <v>3</v>
-      </c>
-      <c r="I57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J57">
-        <v>68</v>
+        <v>134</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
@@ -2115,31 +2139,31 @@
         <v>67</v>
       </c>
       <c r="B58">
-        <v>58.984126984126981</v>
+        <v>56.378205128205131</v>
       </c>
       <c r="C58">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D58">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E58">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F58">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="G58">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="H58">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="I58">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="J58">
-        <v>189</v>
+        <v>156</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
@@ -2147,31 +2171,31 @@
         <v>68</v>
       </c>
       <c r="B59">
-        <v>56.460750853242324</v>
+        <v>62.913907284768214</v>
       </c>
       <c r="C59">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D59">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="E59">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="F59">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="G59">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="H59">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="I59">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="J59">
-        <v>293</v>
+        <v>302</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
@@ -2179,31 +2203,28 @@
         <v>69</v>
       </c>
       <c r="B60">
-        <v>51.916666666666664</v>
+        <v>47.177419354838712</v>
       </c>
       <c r="C60">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D60">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E60">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F60">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G60">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="H60">
-        <v>5</v>
-      </c>
-      <c r="I60">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J60">
-        <v>36</v>
+        <v>62</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
@@ -2211,28 +2232,28 @@
         <v>70</v>
       </c>
       <c r="B61">
-        <v>32.495327102803735</v>
+        <v>43.921052631578945</v>
       </c>
       <c r="C61">
-        <v>89</v>
+        <v>31</v>
       </c>
       <c r="D61">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="E61">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="F61">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="G61">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="H61">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="J61">
-        <v>214</v>
+        <v>190</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
@@ -2240,31 +2261,28 @@
         <v>71</v>
       </c>
       <c r="B62">
-        <v>62.846153846153847</v>
-      </c>
-      <c r="C62">
-        <v>1</v>
+        <v>53.479166666666664</v>
       </c>
       <c r="D62">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E62">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F62">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G62">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="H62">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I62">
         <v>4</v>
       </c>
       <c r="J62">
-        <v>26</v>
+        <v>48</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
@@ -2272,25 +2290,28 @@
         <v>72</v>
       </c>
       <c r="B63">
-        <v>77.027027027027032</v>
+        <v>70.38095238095238</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
       </c>
       <c r="E63">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F63">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G63">
+        <v>4</v>
+      </c>
+      <c r="H63">
+        <v>3</v>
+      </c>
+      <c r="I63">
         <v>7</v>
       </c>
-      <c r="H63">
-        <v>2</v>
-      </c>
-      <c r="I63">
-        <v>19</v>
-      </c>
       <c r="J63">
-        <v>37</v>
+        <v>21</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
@@ -2298,22 +2319,31 @@
         <v>73</v>
       </c>
       <c r="B64">
-        <v>61.428571428571431</v>
+        <v>55.5</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
       </c>
       <c r="D64">
         <v>2</v>
       </c>
+      <c r="E64">
+        <v>5</v>
+      </c>
+      <c r="F64">
+        <v>3</v>
+      </c>
       <c r="G64">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H64">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I64">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J64">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
@@ -2321,28 +2351,22 @@
         <v>26</v>
       </c>
       <c r="B65">
-        <v>60</v>
-      </c>
-      <c r="C65">
-        <v>1</v>
+        <v>70.13333333333334</v>
       </c>
       <c r="D65">
-        <v>1</v>
-      </c>
-      <c r="F65">
+        <v>3</v>
+      </c>
+      <c r="E65">
         <v>2</v>
       </c>
       <c r="G65">
-        <v>2</v>
-      </c>
-      <c r="H65">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I65">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="J65">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
@@ -2350,25 +2374,22 @@
         <v>74</v>
       </c>
       <c r="B66">
-        <v>54.8</v>
+        <v>45</v>
       </c>
       <c r="D66">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E66">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F66">
         <v>6</v>
       </c>
       <c r="G66">
-        <v>6</v>
-      </c>
-      <c r="H66">
         <v>2</v>
       </c>
       <c r="J66">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
@@ -2376,31 +2397,25 @@
         <v>75</v>
       </c>
       <c r="B67">
-        <v>42.056603773584904</v>
+        <v>26.109375</v>
       </c>
       <c r="C67">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="D67">
         <v>10</v>
       </c>
       <c r="E67">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="F67">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G67">
-        <v>3</v>
-      </c>
-      <c r="H67">
-        <v>5</v>
-      </c>
-      <c r="I67">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J67">
-        <v>53</v>
+        <v>64</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
@@ -2408,25 +2423,28 @@
         <v>76</v>
       </c>
       <c r="B68">
-        <v>39.178571428571431</v>
+        <v>46.014285714285712</v>
       </c>
       <c r="C68">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D68">
+        <v>7</v>
+      </c>
+      <c r="E68">
+        <v>35</v>
+      </c>
+      <c r="F68">
         <v>20</v>
       </c>
-      <c r="E68">
-        <v>13</v>
-      </c>
-      <c r="F68">
-        <v>6</v>
-      </c>
       <c r="G68">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="H68">
+        <v>1</v>
       </c>
       <c r="J68">
-        <v>56</v>
+        <v>70</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
@@ -2434,31 +2452,31 @@
         <v>77</v>
       </c>
       <c r="B69">
-        <v>56.894472361809044</v>
+        <v>65.535294117647055</v>
       </c>
       <c r="C69">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D69">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E69">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="F69">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="G69">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H69">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="I69">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="J69">
-        <v>199</v>
+        <v>170</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
@@ -2503,22 +2521,22 @@
         <v>78</v>
       </c>
       <c r="B73">
-        <v>34.823529411764703</v>
-      </c>
-      <c r="C73">
-        <v>6</v>
+        <v>49.6875</v>
       </c>
       <c r="D73">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E73">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="F73">
+        <v>4</v>
       </c>
       <c r="G73">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J73">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
@@ -2526,25 +2544,22 @@
         <v>79</v>
       </c>
       <c r="B74">
-        <v>64.388888888888886</v>
-      </c>
-      <c r="E74">
-        <v>1</v>
+        <v>72.319999999999993</v>
       </c>
       <c r="F74">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G74">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="H74">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="I74">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="J74">
-        <v>18</v>
+        <v>50</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
@@ -2552,28 +2567,28 @@
         <v>80</v>
       </c>
       <c r="B75">
-        <v>55.343434343434346</v>
-      </c>
-      <c r="C75">
-        <v>1</v>
+        <v>59.237885462555063</v>
       </c>
       <c r="D75">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E75">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="F75">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="G75">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="H75">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="I75">
+        <v>1</v>
       </c>
       <c r="J75">
-        <v>198</v>
+        <v>227</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
@@ -2581,31 +2596,22 @@
         <v>81</v>
       </c>
       <c r="B76">
-        <v>50.444444444444443</v>
-      </c>
-      <c r="C76">
-        <v>1</v>
+        <v>48.5</v>
       </c>
       <c r="D76">
+        <v>2</v>
+      </c>
+      <c r="E76">
+        <v>4</v>
+      </c>
+      <c r="F76">
         <v>3</v>
       </c>
-      <c r="E76">
-        <v>1</v>
-      </c>
-      <c r="F76">
-        <v>1</v>
-      </c>
-      <c r="G76">
-        <v>1</v>
-      </c>
       <c r="H76">
         <v>1</v>
       </c>
-      <c r="I76">
-        <v>1</v>
-      </c>
       <c r="J76">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
@@ -2613,25 +2619,31 @@
         <v>82</v>
       </c>
       <c r="B77">
-        <v>42</v>
+        <v>44.542483660130721</v>
       </c>
       <c r="C77">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D77">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="E77">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="F77">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="G77">
-        <v>2</v>
+        <v>11</v>
+      </c>
+      <c r="H77">
+        <v>2</v>
+      </c>
+      <c r="I77">
+        <v>1</v>
       </c>
       <c r="J77">
-        <v>14</v>
+        <v>153</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
@@ -2639,28 +2651,28 @@
         <v>83</v>
       </c>
       <c r="B78">
-        <v>39.102040816326529</v>
-      </c>
-      <c r="C78">
-        <v>7</v>
+        <v>56.625</v>
       </c>
       <c r="D78">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="E78">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F78">
         <v>5</v>
       </c>
       <c r="G78">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="H78">
+        <v>1</v>
+      </c>
+      <c r="I78">
         <v>2</v>
       </c>
       <c r="J78">
-        <v>49</v>
+        <v>24</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
@@ -2668,28 +2680,19 @@
         <v>84</v>
       </c>
       <c r="B79">
-        <v>41.25</v>
-      </c>
-      <c r="C79">
-        <v>5</v>
-      </c>
-      <c r="D79">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="E79">
-        <v>2</v>
-      </c>
-      <c r="F79">
         <v>1</v>
       </c>
       <c r="H79">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I79">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J79">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
@@ -2697,28 +2700,31 @@
         <v>27</v>
       </c>
       <c r="B80">
-        <v>46.786885245901637</v>
+        <v>71.384615384615387</v>
       </c>
       <c r="C80">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D80">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E80">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="F80">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="G80">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="H80">
+        <v>10</v>
       </c>
       <c r="I80">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="J80">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
@@ -2726,31 +2732,28 @@
         <v>85</v>
       </c>
       <c r="B81">
-        <v>45.606060606060609</v>
+        <v>49.396475770925107</v>
       </c>
       <c r="C81">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D81">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="E81">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="F81">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="G81">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="H81">
-        <v>1</v>
-      </c>
-      <c r="I81">
         <v>2</v>
       </c>
       <c r="J81">
-        <v>198</v>
+        <v>227</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
@@ -2758,22 +2761,25 @@
         <v>86</v>
       </c>
       <c r="B82">
-        <v>60.055555555555557</v>
+        <v>63.9</v>
       </c>
       <c r="E82">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F82">
+        <v>11</v>
+      </c>
+      <c r="G82">
+        <v>25</v>
+      </c>
+      <c r="H82">
         <v>8</v>
       </c>
-      <c r="G82">
-        <v>7</v>
-      </c>
-      <c r="H82">
-        <v>2</v>
+      <c r="I82">
+        <v>3</v>
       </c>
       <c r="J82">
-        <v>18</v>
+        <v>50</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
@@ -2781,28 +2787,31 @@
         <v>87</v>
       </c>
       <c r="B83">
-        <v>40.378048780487802</v>
+        <v>40.883333333333333</v>
       </c>
       <c r="C83">
+        <v>10</v>
+      </c>
+      <c r="D83">
+        <v>23</v>
+      </c>
+      <c r="E83">
         <v>14</v>
       </c>
-      <c r="D83">
-        <v>29</v>
-      </c>
-      <c r="E83">
-        <v>16</v>
-      </c>
       <c r="F83">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="G83">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H83">
+        <v>2</v>
+      </c>
+      <c r="I83">
         <v>1</v>
       </c>
       <c r="J83">
-        <v>82</v>
+        <v>60</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
@@ -2810,31 +2819,31 @@
         <v>88</v>
       </c>
       <c r="B84">
-        <v>48.104166666666664</v>
+        <v>52.021164021164019</v>
       </c>
       <c r="C84">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D84">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="E84">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F84">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="G84">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="H84">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="I84">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="J84">
-        <v>144</v>
+        <v>189</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
@@ -2842,31 +2851,31 @@
         <v>89</v>
       </c>
       <c r="B85">
-        <v>49.120370370370374</v>
+        <v>65.494584837545133</v>
       </c>
       <c r="C85">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D85">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="E85">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="F85">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G85">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="H85">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="I85">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="J85">
-        <v>216</v>
+        <v>277</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
@@ -2874,25 +2883,31 @@
         <v>90</v>
       </c>
       <c r="B86">
-        <v>40</v>
+        <v>59.5</v>
       </c>
       <c r="C86">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D86">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E86">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F86">
+        <v>8</v>
+      </c>
+      <c r="G86">
         <v>3</v>
       </c>
-      <c r="G86">
-        <v>2</v>
+      <c r="H86">
+        <v>8</v>
+      </c>
+      <c r="I86">
+        <v>1</v>
       </c>
       <c r="J86">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
@@ -2900,28 +2915,31 @@
         <v>91</v>
       </c>
       <c r="B87">
-        <v>33.6</v>
+        <v>51.507246376811594</v>
       </c>
       <c r="C87">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="D87">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E87">
+        <v>42</v>
+      </c>
+      <c r="F87">
+        <v>60</v>
+      </c>
+      <c r="G87">
+        <v>43</v>
+      </c>
+      <c r="H87">
         <v>15</v>
       </c>
-      <c r="F87">
-        <v>13</v>
-      </c>
-      <c r="G87">
-        <v>9</v>
-      </c>
-      <c r="H87">
-        <v>4</v>
+      <c r="I87">
+        <v>5</v>
       </c>
       <c r="J87">
-        <v>135</v>
+        <v>207</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
@@ -2929,25 +2947,31 @@
         <v>92</v>
       </c>
       <c r="B88">
-        <v>31.666666666666668</v>
+        <v>54.458333333333336</v>
       </c>
       <c r="C88">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D88">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E88">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F88">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G88">
         <v>2</v>
       </c>
+      <c r="H88">
+        <v>5</v>
+      </c>
+      <c r="I88">
+        <v>2</v>
+      </c>
       <c r="J88">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
@@ -2955,19 +2979,25 @@
         <v>28</v>
       </c>
       <c r="B89">
-        <v>34</v>
-      </c>
-      <c r="D89">
-        <v>24</v>
+        <v>63.625</v>
       </c>
       <c r="E89">
+        <v>7</v>
+      </c>
+      <c r="F89">
+        <v>4</v>
+      </c>
+      <c r="G89">
+        <v>10</v>
+      </c>
+      <c r="H89">
+        <v>8</v>
+      </c>
+      <c r="I89">
         <v>3</v>
       </c>
-      <c r="F89">
-        <v>1</v>
-      </c>
       <c r="J89">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
@@ -2975,22 +3005,28 @@
         <v>29</v>
       </c>
       <c r="B90">
-        <v>40.166666666666664</v>
-      </c>
-      <c r="C90">
-        <v>3</v>
+        <v>60.666666666666664</v>
       </c>
       <c r="D90">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E90">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="F90">
+        <v>1</v>
+      </c>
+      <c r="G90">
+        <v>1</v>
       </c>
       <c r="H90">
         <v>1</v>
       </c>
+      <c r="I90">
+        <v>1</v>
+      </c>
       <c r="J90">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
@@ -2998,19 +3034,25 @@
         <v>30</v>
       </c>
       <c r="B91">
-        <v>29.8</v>
+        <v>46.8</v>
       </c>
       <c r="C91">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D91">
         <v>2</v>
       </c>
       <c r="E91">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="F91">
+        <v>2</v>
+      </c>
+      <c r="G91">
+        <v>3</v>
       </c>
       <c r="J91">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
@@ -3018,21 +3060,24 @@
         <v>93</v>
       </c>
       <c r="B92">
-        <v>39.833333333333336</v>
+        <v>45.666666666666664</v>
       </c>
       <c r="C92">
         <v>2</v>
       </c>
       <c r="D92">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E92">
         <v>6</v>
       </c>
       <c r="F92">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G92">
+        <v>1</v>
+      </c>
+      <c r="H92">
         <v>1</v>
       </c>
       <c r="J92">
@@ -3044,22 +3089,28 @@
         <v>94</v>
       </c>
       <c r="B93">
-        <v>52.958333333333336</v>
+        <v>53.065217391304351</v>
+      </c>
+      <c r="D93">
+        <v>9</v>
       </c>
       <c r="E93">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F93">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G93">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="H93">
+        <v>4</v>
       </c>
       <c r="I93">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J93">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
@@ -3067,31 +3118,25 @@
         <v>95</v>
       </c>
       <c r="B94">
-        <v>48.666666666666664</v>
+        <v>33.632653061224488</v>
       </c>
       <c r="C94">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D94">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="E94">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F94">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="G94">
-        <v>7</v>
-      </c>
-      <c r="H94">
-        <v>1</v>
-      </c>
-      <c r="I94">
         <v>1</v>
       </c>
       <c r="J94">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
@@ -3099,31 +3144,31 @@
         <v>96</v>
       </c>
       <c r="B95">
-        <v>55.768000000000001</v>
+        <v>72.368686868686865</v>
       </c>
       <c r="C95">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D95">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E95">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="F95">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="G95">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="H95">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="I95">
-        <v>3</v>
+        <v>78</v>
       </c>
       <c r="J95">
-        <v>125</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>